<commit_message>
workign , macd , incorporated
</commit_message>
<xml_diff>
--- a/backtest_df.xlsx
+++ b/backtest_df.xlsx
@@ -532,7 +532,7 @@
         <v>6.286150000000001</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6298663003663004</v>
+        <v>0.6298663003663002</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
@@ -571,7 +571,7 @@
         <v>6.941025000000001</v>
       </c>
       <c r="J3" t="n">
-        <v>0.6941666666666667</v>
+        <v>0.6941666666666666</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -649,7 +649,7 @@
         <v>7.9675</v>
       </c>
       <c r="J5" t="n">
-        <v>0.8054545454545454</v>
+        <v>0.8054545454545456</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
@@ -727,7 +727,7 @@
         <v>5.964</v>
       </c>
       <c r="J7" t="n">
-        <v>0.6318333333333334</v>
+        <v>0.6318333333333332</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
@@ -883,7 +883,7 @@
         <v>6.17595</v>
       </c>
       <c r="J11" t="n">
-        <v>0.6280238095238094</v>
+        <v>0.6280238095238095</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
@@ -961,7 +961,7 @@
         <v>6.408450000000001</v>
       </c>
       <c r="J13" t="n">
-        <v>0.6414761904761904</v>
+        <v>0.6414761904761903</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
@@ -1078,7 +1078,7 @@
         <v>6.037725</v>
       </c>
       <c r="J16" t="n">
-        <v>0.6293214285714287</v>
+        <v>0.6293214285714286</v>
       </c>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
@@ -1160,7 +1160,7 @@
         <v>7.533</v>
       </c>
       <c r="J18" t="n">
-        <v>0.7774761904761904</v>
+        <v>0.7774761904761905</v>
       </c>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
@@ -1937,7 +1937,7 @@
         <v>6.7133</v>
       </c>
       <c r="J37" t="n">
-        <v>0.6726785714285712</v>
+        <v>0.6726785714285713</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr"/>
@@ -1976,7 +1976,7 @@
         <v>6.09015</v>
       </c>
       <c r="J38" t="n">
-        <v>0.6271785714285713</v>
+        <v>0.6271785714285714</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2597,7 +2597,7 @@
         <v>6.367620000000001</v>
       </c>
       <c r="J53" t="n">
-        <v>0.6370714285714285</v>
+        <v>0.6370714285714286</v>
       </c>
       <c r="K53" t="inlineStr"/>
       <c r="L53" t="inlineStr"/>
@@ -2718,7 +2718,7 @@
         <v>6.219774999999999</v>
       </c>
       <c r="J56" t="n">
-        <v>0.6326071428571428</v>
+        <v>0.6326071428571429</v>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr"/>
@@ -3124,7 +3124,7 @@
         <v>6.987450000000001</v>
       </c>
       <c r="J66" t="n">
-        <v>0.7031043956043955</v>
+        <v>0.7031043956043956</v>
       </c>
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr"/>
@@ -3698,7 +3698,7 @@
         <v>6.06361</v>
       </c>
       <c r="J80" t="n">
-        <v>0.6091428571428572</v>
+        <v>0.6091428571428571</v>
       </c>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr"/>
@@ -3819,7 +3819,7 @@
         <v>6.69</v>
       </c>
       <c r="J83" t="n">
-        <v>0.6697857142857143</v>
+        <v>0.6697857142857141</v>
       </c>
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr"/>
@@ -3983,7 +3983,7 @@
         <v>6.339300000000001</v>
       </c>
       <c r="J87" t="n">
-        <v>0.6351320346320347</v>
+        <v>0.6351320346320346</v>
       </c>
       <c r="K87" t="inlineStr"/>
       <c r="L87" t="inlineStr"/>
@@ -4436,7 +4436,7 @@
         <v>6.39765</v>
       </c>
       <c r="J98" t="n">
-        <v>0.6441944444444444</v>
+        <v>0.6441944444444445</v>
       </c>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr"/>
@@ -4557,7 +4557,7 @@
         <v>6.3847</v>
       </c>
       <c r="J101" t="n">
-        <v>0.6533333333333334</v>
+        <v>0.6533333333333331</v>
       </c>
       <c r="K101" t="inlineStr"/>
       <c r="L101" t="inlineStr"/>
@@ -4803,7 +4803,7 @@
         <v>5.990100000000001</v>
       </c>
       <c r="J107" t="n">
-        <v>0.6156904761904761</v>
+        <v>0.6156904761904762</v>
       </c>
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr"/>
@@ -5088,7 +5088,7 @@
         <v>6.58425</v>
       </c>
       <c r="J114" t="n">
-        <v>0.6966666666666668</v>
+        <v>0.6966666666666669</v>
       </c>
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
@@ -5334,7 +5334,7 @@
         <v>7.074375</v>
       </c>
       <c r="J120" t="n">
-        <v>0.7133095238095237</v>
+        <v>0.7133095238095238</v>
       </c>
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr"/>
@@ -5455,7 +5455,7 @@
         <v>6.05836</v>
       </c>
       <c r="J123" t="n">
-        <v>0.6070674603174604</v>
+        <v>0.6070674603174603</v>
       </c>
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr"/>
@@ -5537,7 +5537,7 @@
         <v>6.4396</v>
       </c>
       <c r="J125" t="n">
-        <v>0.6551349206349208</v>
+        <v>0.6551349206349206</v>
       </c>
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr"/>
@@ -5701,7 +5701,7 @@
         <v>6.330870000000001</v>
       </c>
       <c r="J129" t="n">
-        <v>0.6381666666666667</v>
+        <v>0.6381666666666665</v>
       </c>
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr"/>
@@ -5783,7 +5783,7 @@
         <v>6.038399999999999</v>
       </c>
       <c r="J131" t="n">
-        <v>0.6247142857142857</v>
+        <v>0.6247142857142858</v>
       </c>
       <c r="K131" t="inlineStr"/>
       <c r="L131" t="inlineStr"/>
@@ -5947,7 +5947,7 @@
         <v>6.4152</v>
       </c>
       <c r="J135" t="n">
-        <v>0.6512619047619048</v>
+        <v>0.6512619047619047</v>
       </c>
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr"/>
@@ -6158,7 +6158,7 @@
         <v>6.10575</v>
       </c>
       <c r="J140" t="n">
-        <v>0.6469047619047619</v>
+        <v>0.6469047619047618</v>
       </c>
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr"/>
@@ -6236,7 +6236,7 @@
         <v>5.5905</v>
       </c>
       <c r="J142" t="n">
-        <v>0.6121547619047618</v>
+        <v>0.6121547619047619</v>
       </c>
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr"/>
@@ -6275,7 +6275,7 @@
         <v>6.229125</v>
       </c>
       <c r="J143" t="n">
-        <v>0.6620119047619046</v>
+        <v>0.6620119047619047</v>
       </c>
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr"/>
@@ -6314,7 +6314,7 @@
         <v>5.984125</v>
       </c>
       <c r="J144" t="n">
-        <v>0.6011904761904762</v>
+        <v>0.6011904761904761</v>
       </c>
       <c r="K144" t="inlineStr"/>
       <c r="L144" t="inlineStr"/>
@@ -6439,7 +6439,7 @@
         <v>6.30504</v>
       </c>
       <c r="J147" t="n">
-        <v>0.6326666666666667</v>
+        <v>0.6326666666666666</v>
       </c>
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr"/>
@@ -6560,7 +6560,7 @@
         <v>5.8734</v>
       </c>
       <c r="J150" t="n">
-        <v>0.672142857142857</v>
+        <v>0.6721428571428573</v>
       </c>
       <c r="K150" t="inlineStr"/>
       <c r="L150" t="inlineStr"/>
@@ -7013,7 +7013,7 @@
         <v>7.784925</v>
       </c>
       <c r="J161" t="n">
-        <v>0.7903333333333334</v>
+        <v>0.7903333333333333</v>
       </c>
       <c r="K161" t="inlineStr"/>
       <c r="L161" t="inlineStr"/>
@@ -7302,7 +7302,7 @@
         <v>6.628875</v>
       </c>
       <c r="J168" t="n">
-        <v>0.664611111111111</v>
+        <v>0.6646111111111113</v>
       </c>
       <c r="K168" t="inlineStr"/>
       <c r="L168" t="inlineStr"/>
@@ -7341,7 +7341,7 @@
         <v>6.02875</v>
       </c>
       <c r="J169" t="n">
-        <v>0.6393015873015875</v>
+        <v>0.6393015873015874</v>
       </c>
       <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr"/>
@@ -7630,7 +7630,7 @@
         <v>6.73508</v>
       </c>
       <c r="J176" t="n">
-        <v>0.6750595238095238</v>
+        <v>0.6750595238095236</v>
       </c>
       <c r="K176" t="inlineStr"/>
       <c r="L176" t="inlineStr"/>
@@ -7669,7 +7669,7 @@
         <v>6.109375</v>
       </c>
       <c r="J177" t="n">
-        <v>0.6176825396825395</v>
+        <v>0.6176825396825396</v>
       </c>
       <c r="K177" t="inlineStr"/>
       <c r="L177" t="inlineStr"/>
@@ -7708,7 +7708,7 @@
         <v>6.4416</v>
       </c>
       <c r="J178" t="n">
-        <v>0.6551666666666667</v>
+        <v>0.6551666666666668</v>
       </c>
       <c r="K178" t="inlineStr"/>
       <c r="L178" t="inlineStr"/>
@@ -7872,7 +7872,7 @@
         <v>6.270960000000001</v>
       </c>
       <c r="J182" t="n">
-        <v>0.6368809523809524</v>
+        <v>0.6368809523809523</v>
       </c>
       <c r="K182" t="inlineStr"/>
       <c r="L182" t="inlineStr"/>
@@ -8364,7 +8364,7 @@
         <v>5.436299999999999</v>
       </c>
       <c r="J194" t="n">
-        <v>0.6139047619047618</v>
+        <v>0.613904761904762</v>
       </c>
       <c r="K194" t="inlineStr"/>
       <c r="L194" t="inlineStr"/>
@@ -8485,7 +8485,7 @@
         <v>6.09735</v>
       </c>
       <c r="J197" t="n">
-        <v>0.6266666666666667</v>
+        <v>0.6266666666666666</v>
       </c>
       <c r="K197" t="inlineStr"/>
       <c r="L197" t="inlineStr"/>
@@ -8567,7 +8567,7 @@
         <v>6.450675</v>
       </c>
       <c r="J199" t="n">
-        <v>0.6512380952380953</v>
+        <v>0.6512380952380954</v>
       </c>
       <c r="K199" t="inlineStr"/>
       <c r="L199" t="inlineStr"/>
@@ -8688,7 +8688,7 @@
         <v>7.40675</v>
       </c>
       <c r="J202" t="n">
-        <v>0.7433809523809524</v>
+        <v>0.7433809523809525</v>
       </c>
       <c r="K202" t="inlineStr"/>
       <c r="L202" t="inlineStr"/>
@@ -9219,7 +9219,7 @@
         <v>6.153424999999999</v>
       </c>
       <c r="J215" t="n">
-        <v>0.6155119047619046</v>
+        <v>0.6155119047619045</v>
       </c>
       <c r="K215" t="inlineStr"/>
       <c r="L215" t="inlineStr"/>
@@ -9301,7 +9301,7 @@
         <v>6.816974999999999</v>
       </c>
       <c r="J217" t="n">
-        <v>0.7001666666666666</v>
+        <v>0.7001666666666665</v>
       </c>
       <c r="K217" t="inlineStr"/>
       <c r="L217" t="inlineStr"/>
@@ -9426,7 +9426,7 @@
         <v>6.65741</v>
       </c>
       <c r="J220" t="n">
-        <v>0.6710476190476189</v>
+        <v>0.671047619047619</v>
       </c>
       <c r="K220" t="inlineStr"/>
       <c r="L220" t="inlineStr"/>
@@ -9465,7 +9465,7 @@
         <v>6.02301</v>
       </c>
       <c r="J221" t="n">
-        <v>0.6104285714285714</v>
+        <v>0.6104285714285715</v>
       </c>
       <c r="K221" t="inlineStr"/>
       <c r="L221" t="inlineStr"/>
@@ -9629,7 +9629,7 @@
         <v>6.23616</v>
       </c>
       <c r="J225" t="n">
-        <v>0.6356904761904763</v>
+        <v>0.6356904761904761</v>
       </c>
       <c r="K225" t="inlineStr"/>
       <c r="L225" t="inlineStr"/>
@@ -9750,7 +9750,7 @@
         <v>6.912675</v>
       </c>
       <c r="J228" t="n">
-        <v>0.7041666666666666</v>
+        <v>0.7041666666666667</v>
       </c>
       <c r="K228" t="inlineStr"/>
       <c r="L228" t="inlineStr"/>
@@ -10207,7 +10207,7 @@
         <v>6.472200000000001</v>
       </c>
       <c r="J239" t="n">
-        <v>0.6660119047619045</v>
+        <v>0.6660119047619046</v>
       </c>
       <c r="K239" t="inlineStr"/>
       <c r="L239" t="inlineStr"/>
@@ -10496,7 +10496,7 @@
         <v>5.932</v>
       </c>
       <c r="J246" t="n">
-        <v>0.6407380952380951</v>
+        <v>0.6407380952380953</v>
       </c>
       <c r="K246" t="inlineStr"/>
       <c r="L246" t="inlineStr"/>
@@ -10742,7 +10742,7 @@
         <v>5.60175</v>
       </c>
       <c r="J252" t="n">
-        <v>0.602095238095238</v>
+        <v>0.6020952380952379</v>
       </c>
       <c r="K252" t="inlineStr"/>
       <c r="L252" t="inlineStr"/>
@@ -10781,7 +10781,7 @@
         <v>7.200900000000001</v>
       </c>
       <c r="J253" t="n">
-        <v>0.7234523809523811</v>
+        <v>0.7234523809523812</v>
       </c>
       <c r="K253" t="inlineStr"/>
       <c r="L253" t="inlineStr"/>
@@ -10863,7 +10863,7 @@
         <v>6.24685</v>
       </c>
       <c r="J255" t="n">
-        <v>0.6293571428571428</v>
+        <v>0.6293571428571429</v>
       </c>
       <c r="K255" t="inlineStr"/>
       <c r="L255" t="inlineStr"/>
@@ -11234,7 +11234,7 @@
         <v>6.844</v>
       </c>
       <c r="J264" t="n">
-        <v>0.7008333333333333</v>
+        <v>0.7008333333333334</v>
       </c>
       <c r="K264" t="inlineStr"/>
       <c r="L264" t="inlineStr"/>
@@ -11437,7 +11437,7 @@
         <v>5.487</v>
       </c>
       <c r="J269" t="n">
-        <v>0.6036428571428571</v>
+        <v>0.603642857142857</v>
       </c>
       <c r="K269" t="inlineStr"/>
       <c r="L269" t="inlineStr"/>
@@ -11558,7 +11558,7 @@
         <v>5.3598</v>
       </c>
       <c r="J272" t="n">
-        <v>0.6001547619047619</v>
+        <v>0.6001547619047618</v>
       </c>
       <c r="K272" t="inlineStr"/>
       <c r="L272" t="inlineStr"/>
@@ -12015,7 +12015,7 @@
         <v>6.080799999999999</v>
       </c>
       <c r="J283" t="n">
-        <v>0.6326904761904762</v>
+        <v>0.6326904761904761</v>
       </c>
       <c r="K283" t="inlineStr"/>
       <c r="L283" t="inlineStr"/>
@@ -12093,7 +12093,7 @@
         <v>6.222825</v>
       </c>
       <c r="J285" t="n">
-        <v>0.63</v>
+        <v>0.6299999999999999</v>
       </c>
       <c r="K285" t="inlineStr"/>
       <c r="L285" t="inlineStr"/>
@@ -12382,7 +12382,7 @@
         <v>5.7323</v>
       </c>
       <c r="J292" t="n">
-        <v>0.650690476190476</v>
+        <v>0.6506904761904763</v>
       </c>
       <c r="K292" t="inlineStr"/>
       <c r="L292" t="inlineStr"/>
@@ -12464,7 +12464,7 @@
         <v>6.7367</v>
       </c>
       <c r="J294" t="n">
-        <v>0.6763095238095239</v>
+        <v>0.6763095238095238</v>
       </c>
       <c r="K294" t="inlineStr"/>
       <c r="L294" t="inlineStr"/>
@@ -12542,7 +12542,7 @@
         <v>6.4476</v>
       </c>
       <c r="J296" t="n">
-        <v>0.6826190476190477</v>
+        <v>0.6826190476190476</v>
       </c>
       <c r="K296" t="inlineStr"/>
       <c r="L296" t="inlineStr"/>
@@ -13124,7 +13124,7 @@
         <v>7.726500000000001</v>
       </c>
       <c r="J310" t="n">
-        <v>0.8068333333333334</v>
+        <v>0.8068333333333332</v>
       </c>
       <c r="K310" t="inlineStr"/>
       <c r="L310" t="inlineStr"/>
@@ -13417,7 +13417,7 @@
         <v>5.1645</v>
       </c>
       <c r="J317" t="n">
-        <v>0.6033333333333332</v>
+        <v>0.6033333333333333</v>
       </c>
       <c r="K317" t="inlineStr"/>
       <c r="L317" t="inlineStr"/>
@@ -13952,7 +13952,7 @@
         <v>6.02446</v>
       </c>
       <c r="J330" t="n">
-        <v>0.6033690476190475</v>
+        <v>0.6033690476190476</v>
       </c>
       <c r="K330" t="inlineStr"/>
       <c r="L330" t="inlineStr"/>
@@ -14034,7 +14034,7 @@
         <v>6.689480000000001</v>
       </c>
       <c r="J332" t="n">
-        <v>0.6695555555555555</v>
+        <v>0.6695555555555557</v>
       </c>
       <c r="K332" t="inlineStr"/>
       <c r="L332" t="inlineStr"/>
@@ -14155,7 +14155,7 @@
         <v>6.041525000000001</v>
       </c>
       <c r="J335" t="n">
-        <v>0.6127142857142858</v>
+        <v>0.6127142857142855</v>
       </c>
       <c r="K335" t="inlineStr"/>
       <c r="L335" t="inlineStr"/>
@@ -14319,7 +14319,7 @@
         <v>6.281099999999999</v>
       </c>
       <c r="J339" t="n">
-        <v>0.6384761904761905</v>
+        <v>0.6384761904761904</v>
       </c>
       <c r="K339" t="inlineStr"/>
       <c r="L339" t="inlineStr"/>
@@ -14940,7 +14940,7 @@
         <v>6.765000000000001</v>
       </c>
       <c r="J354" t="n">
-        <v>0.6869047619047618</v>
+        <v>0.6869047619047619</v>
       </c>
       <c r="K354" t="inlineStr"/>
       <c r="L354" t="inlineStr"/>
@@ -15018,7 +15018,7 @@
         <v>6.8145</v>
       </c>
       <c r="J356" t="n">
-        <v>0.7127619047619045</v>
+        <v>0.7127619047619046</v>
       </c>
       <c r="K356" t="inlineStr"/>
       <c r="L356" t="inlineStr"/>
@@ -16002,7 +16002,7 @@
         <v>6.373600000000001</v>
       </c>
       <c r="J380" t="n">
-        <v>0.6511190476190477</v>
+        <v>0.6511190476190475</v>
       </c>
       <c r="K380" t="inlineStr"/>
       <c r="L380" t="inlineStr"/>

</xml_diff>